<commit_message>
changed some stuff in current invoice so that it uses payload instead of parts, not sure if this should be universally applied or not
</commit_message>
<xml_diff>
--- a/Vendors - Monthly.xlsx
+++ b/Vendors - Monthly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B17001B-016F-4AF7-9B73-D3C21184A18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8962C4-7827-4D72-96E8-B6280001A43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Vendors</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Turek &amp; Sons, LLC</t>
+  </si>
+  <si>
+    <t>Holcim</t>
   </si>
 </sst>
 </file>
@@ -447,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9267CA-59CB-45E5-B346-87C338D47B3D}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +480,7 @@
         <v>4</v>
       </c>
       <c r="I1">
-        <v>33304</v>
+        <v>33325</v>
       </c>
       <c r="K1" t="s">
         <v>18</v>
@@ -487,6 +490,9 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" t="s">
         <v>3</v>
       </c>
@@ -503,6 +509,9 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -535,13 +544,16 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
       <c r="G8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
@@ -549,10 +561,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
@@ -560,7 +569,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" t="s">
         <v>3</v>
@@ -568,10 +577,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G12" t="s">
         <v>3</v>
@@ -579,32 +585,29 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
         <v>3</v>
       </c>
@@ -651,6 +654,11 @@
     </row>
     <row r="25" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added better email retrieval with only more recent emails
</commit_message>
<xml_diff>
--- a/Vendors - Monthly.xlsx
+++ b/Vendors - Monthly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CEFB64-ECC3-4CE2-8627-22FA400D749C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E3C6AB-041C-4D31-8D6A-D731E68FD69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19020" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>Vendors</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Lakeshore Recyling</t>
+  </si>
+  <si>
+    <t>Atlas Crane Service</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9267CA-59CB-45E5-B346-87C338D47B3D}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +489,7 @@
         <v>4</v>
       </c>
       <c r="I1">
-        <v>33390</v>
+        <v>33396</v>
       </c>
       <c r="K1" t="s">
         <v>18</v>
@@ -496,6 +499,9 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" t="s">
         <v>3</v>
       </c>
@@ -510,7 +516,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
@@ -518,7 +524,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -526,7 +535,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
@@ -534,10 +543,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
         <v>3</v>
@@ -545,7 +551,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
         <v>3</v>
@@ -553,7 +559,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
@@ -561,34 +570,28 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
       </c>
       <c r="G13" t="s">
         <v>3</v>
@@ -596,7 +599,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G14" t="s">
         <v>3</v>
@@ -604,10 +607,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G15" t="s">
         <v>3</v>
@@ -615,26 +615,29 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="G18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
         <v>3</v>
       </c>
@@ -681,6 +684,11 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added float type casting for AIA forms
</commit_message>
<xml_diff>
--- a/Vendors - Monthly.xlsx
+++ b/Vendors - Monthly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB599C5-6E42-4E63-A980-45C3ACA89F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644D8EF0-F6C2-48D9-AECC-7422E3906CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
+    <workbookView xWindow="39045" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>Vendors</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Hernandez Lawn Service</t>
+  </si>
+  <si>
+    <t>Carlisle Roofing Systems Inc.</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9267CA-59CB-45E5-B346-87C338D47B3D}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="I1">
-        <v>33423</v>
+        <v>33439</v>
       </c>
       <c r="K1" t="s">
         <v>18</v>
@@ -518,6 +521,9 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -540,7 +546,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
       </c>
       <c r="G7" t="s">
         <v>3</v>
@@ -548,10 +557,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
         <v>3</v>
@@ -559,7 +565,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
@@ -567,10 +573,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
@@ -578,7 +581,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
         <v>3</v>
@@ -586,28 +589,34 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="G13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="G14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
+      <c r="B15" t="s">
+        <v>3</v>
       </c>
       <c r="G15" t="s">
         <v>3</v>
@@ -615,7 +624,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
       </c>
       <c r="G16" t="s">
         <v>3</v>
@@ -623,7 +635,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -634,29 +646,32 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="G20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
         <v>3</v>
       </c>
@@ -703,6 +718,11 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed scanning programs lol thank god!!!!!!
</commit_message>
<xml_diff>
--- a/Vendors - Monthly.xlsx
+++ b/Vendors - Monthly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B506C344-5098-4B53-9478-DC5D8CA2CFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D421ABA-0676-49BF-9ECE-5863BBC3968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>Vendors</t>
   </si>
@@ -468,7 +468,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="I1">
-        <v>33516</v>
+        <v>33562</v>
       </c>
       <c r="K1" t="s">
         <v>18</v>
@@ -505,9 +505,6 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="G2" t="s">
         <v>3</v>
       </c>
@@ -564,6 +561,9 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
       <c r="G9" t="s">
         <v>3</v>
       </c>
@@ -572,9 +572,6 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
       <c r="G10" t="s">
         <v>3</v>
       </c>
@@ -612,9 +609,6 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
       <c r="G15" t="s">
         <v>3</v>
       </c>
@@ -644,6 +638,9 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
       </c>
       <c r="G18" t="s">
         <v>3</v>

</xml_diff>